<commit_message>
20251217 Review December 1612 done
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202512/Developed Market.xlsx
+++ b/GUI + Reviews/202512/Developed Market.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202512\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202512/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D503818E-1B60-45D9-970D-9BEC219AC1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D503818E-1B60-45D9-970D-9BEC219AC1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2494B4E6-A221-48EE-8E54-823A2B027EC5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5A833336-74F3-4282-AA56-06FEBA375784}"/>
+    <workbookView xWindow="-315" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{5A833336-74F3-4282-AA56-06FEBA375784}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14295,20 +14295,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14098694-52FD-4E33-9ABD-FC70E09F5F9E}" name="Universe" displayName="Universe" ref="A1:K1801" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14098694-52FD-4E33-9ABD-FC70E09F5F9E}" name="Universe" displayName="Universe" ref="A1:K1801" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K1801" xr:uid="{14098694-52FD-4E33-9ABD-FC70E09F5F9E}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CFB3C9D6-1DE6-4E4D-854A-DFFA6C6A4E6F}" name="Rank" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{22DA294F-95AB-4307-B7FD-73EBAC7F6EF9}" name="Ticker" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{8CFFCC8C-1003-4180-A56E-7ABB2BCA8603}" name="Name" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{34C78790-2CE9-496D-8DF0-DE032A5D5C18}" name="ISIN" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{17264079-E2E4-4D85-94AA-7E35804E9940}" name="MIC" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{ECCE2221-3DC0-4B96-A738-156BEBC316C1}" name="NOSH" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{59AFD3EA-12CA-43C7-82EF-B6A281BC51A3}" name="Price (EUR) " dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{178CD7DA-992E-48BF-84B3-3D0109654F60}" name="Currency (Local)" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{4F1E1E7D-60C9-4C2A-9398-8C5097CFE74C}" name="Mcap in EUR" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{54C74F0E-1A13-4FC9-8DD8-E7F6F03D6308}" name="index" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{1A494A0A-0294-4A44-B890-1E1A944FF817}" name="3 months ADTV" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CFB3C9D6-1DE6-4E4D-854A-DFFA6C6A4E6F}" name="Rank" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{22DA294F-95AB-4307-B7FD-73EBAC7F6EF9}" name="Ticker" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{8CFFCC8C-1003-4180-A56E-7ABB2BCA8603}" name="Name" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{34C78790-2CE9-496D-8DF0-DE032A5D5C18}" name="ISIN" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{17264079-E2E4-4D85-94AA-7E35804E9940}" name="MIC" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{ECCE2221-3DC0-4B96-A738-156BEBC316C1}" name="NOSH" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{59AFD3EA-12CA-43C7-82EF-B6A281BC51A3}" name="Price (EUR) " dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{178CD7DA-992E-48BF-84B3-3D0109654F60}" name="Currency (Local)" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4F1E1E7D-60C9-4C2A-9398-8C5097CFE74C}" name="Mcap in EUR" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{54C74F0E-1A13-4FC9-8DD8-E7F6F03D6308}" name="index" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{1A494A0A-0294-4A44-B890-1E1A944FF817}" name="3 months ADTV" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14633,7 +14633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC12ED06-37CF-46ED-9A79-DF1CDF88EC2B}">
   <dimension ref="A1:K1801"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1406" workbookViewId="0">
+      <selection activeCell="E1422" sqref="E1422"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -64542,7 +64544,7 @@
         <v>53</v>
       </c>
       <c r="F1426" s="1">
-        <v>2637743772</v>
+        <v>2344661130</v>
       </c>
       <c r="G1426" s="1">
         <v>49.238591399999997</v>

</xml_diff>